<commit_message>
Uploaded on 20-May-2023 before Thesis submission
Uploaded on 20-May-2023 before Thesis submission
</commit_message>
<xml_diff>
--- a/IIoT readiness Assessment.xlsx
+++ b/IIoT readiness Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSC Soln Architect\COMP9028 - Comp Research Project Implem\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71948DF-5780-48E4-AD05-CC704038EB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6032A87-70E2-416B-A21C-FAA56AD70E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>No real issues , just want to progress with IIoT connectivity</t>
+  </si>
+  <si>
+    <t>Product Number, Pallets, From/To locations</t>
+  </si>
+  <si>
+    <t>Product Number, Pallets</t>
   </si>
 </sst>
 </file>
@@ -160,7 +166,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -193,8 +199,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -235,10 +241,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -578,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:M6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -754,6 +760,9 @@
       <c r="L4" t="s">
         <v>21</v>
       </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -794,7 +803,7 @@
         <v>41</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -836,7 +845,7 @@
         <v>41</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>